<commit_message>
hackathon changes-altered framework and increaed scope for test cases
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TC01_LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="TC02_SignUp" sheetId="2" r:id="rId2"/>
+    <sheet name="TC03_CreateTeam" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -42,13 +42,52 @@
     <t>Password</t>
   </si>
   <si>
-    <t>TestUser</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
+    <t>pradeep</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testuser123</t>
+  </si>
+  <si>
+    <t>Automationuser</t>
+  </si>
+  <si>
+    <t>AutomationUser</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liked, Learned, Lacked, Longed for </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anchors, Engines </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drop,Add,Keep,Improve </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Future considerations,Lessons learned, Accomplishments,Problem areas </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mad, Sad, Glad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start, More of, Continue, Less of, Stop </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start, Stop </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start, Stop, Continue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wishes, Risks, Appreciations, Puzzles </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Design your own </t>
   </si>
 </sst>
 </file>
@@ -426,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,28 +477,37 @@
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -468,6 +516,7 @@
     <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -475,11 +524,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -494,31 +548,94 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>